<commit_message>
Riesgos de un proyecto de tics pdf
</commit_message>
<xml_diff>
--- a/17_Proyectos_de_innovacion/Riesgos de un proyecto.xlsx
+++ b/17_Proyectos_de_innovacion/Riesgos de un proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\9 semestre\17_Proyectos_de_innovacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA508BAA-7162-4F48-9201-831B01DAD9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE397A62-6B64-4488-B025-8EC32573C90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BCF61DE-45B9-40A9-ADAE-70508B1836C7}"/>
   </bookViews>
@@ -72,19 +72,25 @@
     <t>Omision de actividades</t>
   </si>
   <si>
-    <t xml:space="preserve">Hacer que todo el equipo este conciente de los cambios, evaluar cuales son los mas importantes y empezar a trabajar en ellos antes de continuar con otros requerimientos  </t>
-  </si>
-  <si>
     <t>Medidas a tomar</t>
   </si>
   <si>
-    <t>Dedicar equipos que puedan brindar apoyo y contenido para aquellos que tienen alguna duda, con la aplicacion, motor, requerimientos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar testings al finalizar un requerimiento que se puede considerar grande, y no al final del sprint en el perioso de lanzamiento a produccion  </t>
-  </si>
-  <si>
-    <t>Dependiendo el tipo de proyecto, podemos pedir mas financiamiento, o bien pedir apoyo por otros medios como donaciones o incluso dejar que la empresa sea absorvida por una empresa mas grande</t>
+    <t>Dependiendo el tipo de proyecto, podemos pedir mas financiamiento, 
+o bien pedir apoyo por otros medios como donaciones o incluso dejar
+ que la empresa sea absorvida por una empresa mas grande</t>
+  </si>
+  <si>
+    <t>Dedicar equipos que puedan brindar apoyo y contenido para aquellos 
+que tienen alguna duda, con la aplicacion, motor, requerimientos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer que todo el equipo este conciente de los cambios, evaluar
+cuales son los mas importantes y empezar a trabajar en ellos antes 
+de continuar con otros requerimientos  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar testings al finalizar un requerimiento que se puede considerar
+ grande, y no al final del sprint en el periodo de lanzamiento a produccion  </t>
   </si>
 </sst>
 </file>
@@ -149,10 +155,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,15 +514,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4FD73F-47CE-49E3-BE35-86178CA9A892}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="177" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,7 +551,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -552,11 +561,11 @@
       <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -566,8 +575,8 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,7 +591,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -592,8 +601,8 @@
       <c r="C6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,7 +617,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -618,8 +627,8 @@
       <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>